<commit_message>
Update BOM-speeduino v0.4.3 compatible PCB for m50tu rev2.1.xlsx
</commit_message>
<xml_diff>
--- a/m50,m40,m60 Pnp/Rev 2.1/BOM-speeduino v0.4.3 compatible PCB for m50tu rev2.1.xlsx
+++ b/m50,m40,m60 Pnp/Rev 2.1/BOM-speeduino v0.4.3 compatible PCB for m50tu rev2.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pasi\Documents\GitHub\Speeduino-M5x-PCBs\m50,m40,m60 Pnp\Rev 2.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3065A020-748B-4348-A03D-DC1869248C3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A936BF54-8B6D-434B-BE2F-ED710D5E97D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1163,6 +1163,27 @@
   </si>
   <si>
     <r>
+      <t>R2,R4,R6,R8,R22,R41,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Liberation Sans"/>
+      </rPr>
+      <t>R64</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Liberation Sans"/>
+      </rPr>
+      <t>,R72,R77,R78</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t>R10,R13,R16,R19,R21,R23,R24,R29,R30,</t>
     </r>
     <r>
@@ -1195,36 +1216,7 @@
         <color rgb="FF000000"/>
         <rFont val="Liberation Sans"/>
       </rPr>
-      <t>,R62</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Liberation Sans"/>
-      </rPr>
-      <t>,R71,R73,R79</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>R2,R4,R6,R8,R22,R41,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Liberation Sans"/>
-      </rPr>
-      <t>R64</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Liberation Sans"/>
-      </rPr>
-      <t>,R72,R77,R78</t>
+      <t>,R60,R62,R71,R73,R79</t>
     </r>
   </si>
 </sst>
@@ -2008,7 +2000,7 @@
   <dimension ref="A1:S60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3670,10 +3662,10 @@
     <row r="32" spans="1:19" ht="26.25" thickBot="1">
       <c r="A32" s="17">
         <f>LEN(B32)-LEN(SUBSTITUTE(B32,",",""))+1</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>43</v>
@@ -3703,28 +3695,28 @@
       </c>
       <c r="M32" s="6">
         <f t="shared" ref="M32:M39" si="8">K32*A32</f>
-        <v>1.3199999999999998</v>
+        <v>1.38</v>
       </c>
       <c r="N32" s="6">
         <f t="shared" ref="N32:N39" si="9">L32*A32</f>
-        <v>2.42</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="O32" s="4"/>
       <c r="P32" s="4" t="str">
         <f t="shared" ref="P32:P41" si="10">IF(NOT(I32=""),A32&amp;","&amp;I32,"")</f>
-        <v>22,1.00KXBK-ND</v>
+        <v>23,1.00KXBK-ND</v>
       </c>
       <c r="Q32" t="str">
         <f t="shared" ref="Q32:Q39" si="11">"Resistor - " &amp; A32&amp;"x "&amp;C32</f>
-        <v>Resistor - 22x 1k</v>
+        <v>Resistor - 23x 1k</v>
       </c>
       <c r="R32" t="str">
         <f t="shared" ref="R32:R41" si="12">IF(NOT(J32=""),J32&amp;"|"&amp;A32,"")</f>
-        <v>603-MFR-25FBF52-1K|22</v>
+        <v>603-MFR-25FBF52-1K|23</v>
       </c>
       <c r="S32" t="str">
         <f t="shared" ref="S32:S41" si="13">H32&amp;" "&amp;A32</f>
-        <v>MFR-25FBF52-1K 22</v>
+        <v>MFR-25FBF52-1K 23</v>
       </c>
     </row>
     <row r="33" spans="1:19" ht="16.5" thickBot="1">
@@ -3795,7 +3787,7 @@
         <v>10</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C34" s="3">
         <v>470</v>
@@ -4844,11 +4836,11 @@
       <c r="L54" s="1"/>
       <c r="M54" s="10">
         <f>SUM(M3:M52)</f>
-        <v>111.63</v>
+        <v>111.69</v>
       </c>
       <c r="N54" s="10">
         <f>SUM(N3:N52)</f>
-        <v>129.70099999999999</v>
+        <v>129.81100000000001</v>
       </c>
       <c r="O54" s="9" t="s">
         <v>65</v>

</xml_diff>